<commit_message>
lab6 koniec i lab 5 poprawka
</commit_message>
<xml_diff>
--- a/lab6/xlsx5.xlsx
+++ b/lab6/xlsx5.xlsx
@@ -3,16 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059BE943-04D9-468F-A0ED-E1992D69E2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0A69C3-9D99-458D-B9B1-EC18C4DB065F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela 1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabela 2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2109,7 +2122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
@@ -7875,8 +7888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7918,1314 +7931,2930 @@
       <c r="A2" s="11">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="12"/>
+      <c r="B2" s="4">
+        <v>914.59402599999999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>42.571857000000001</v>
+      </c>
+      <c r="D2" s="4">
+        <v>196.504131</v>
+      </c>
+      <c r="E2" s="21">
+        <v>64.255111999999997</v>
+      </c>
+      <c r="F2" s="4">
+        <v>5.6838389999999999</v>
+      </c>
+      <c r="G2" s="26">
+        <v>0.50378100000000003</v>
+      </c>
+      <c r="H2" s="3">
+        <v>15.089634999999999</v>
+      </c>
+      <c r="I2" s="12">
+        <v>508</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>0.01</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="9"/>
+      <c r="B3" s="5">
+        <v>671.48659599999996</v>
+      </c>
+      <c r="C3" s="1">
+        <v>29.967718999999999</v>
+      </c>
+      <c r="D3" s="5">
+        <v>196.52386200000001</v>
+      </c>
+      <c r="E3" s="22">
+        <v>64.188952999999998</v>
+      </c>
+      <c r="F3" s="5">
+        <v>5.6727100000000004</v>
+      </c>
+      <c r="G3" s="24">
+        <v>0.50601399999999996</v>
+      </c>
+      <c r="H3" s="1">
+        <v>15.137860999999999</v>
+      </c>
+      <c r="I3" s="9">
+        <v>642</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>0.02</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="9"/>
+      <c r="B4" s="5">
+        <v>661.48898699999995</v>
+      </c>
+      <c r="C4" s="1">
+        <v>16.549696999999998</v>
+      </c>
+      <c r="D4" s="5">
+        <v>196.54380699999999</v>
+      </c>
+      <c r="E4" s="22">
+        <v>64.122281999999998</v>
+      </c>
+      <c r="F4" s="5">
+        <v>5.6615070000000003</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0.50827599999999995</v>
+      </c>
+      <c r="H4" s="1">
+        <v>15.186669999999999</v>
+      </c>
+      <c r="I4" s="9">
+        <v>753</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>0.03</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="9"/>
+      <c r="B5" s="5">
+        <v>442.53641399999998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>20.650061999999998</v>
+      </c>
+      <c r="D5" s="5">
+        <v>196.56387100000001</v>
+      </c>
+      <c r="E5" s="22">
+        <v>64.055114000000003</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5.6502290000000004</v>
+      </c>
+      <c r="G5" s="24">
+        <v>0.51056800000000002</v>
+      </c>
+      <c r="H5" s="1">
+        <v>15.236050000000001</v>
+      </c>
+      <c r="I5" s="9">
+        <v>765</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>0.04</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="9"/>
+      <c r="B6" s="5">
+        <v>970.84927800000003</v>
+      </c>
+      <c r="C6" s="1">
+        <v>37.262613000000002</v>
+      </c>
+      <c r="D6" s="5">
+        <v>196.58404899999999</v>
+      </c>
+      <c r="E6" s="22">
+        <v>63.987431999999998</v>
+      </c>
+      <c r="F6" s="5">
+        <v>5.6388740000000004</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0.51288900000000004</v>
+      </c>
+      <c r="H6" s="1">
+        <v>15.286016999999999</v>
+      </c>
+      <c r="I6" s="9">
+        <v>639</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>0.05</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="9"/>
+      <c r="B7" s="5">
+        <v>981.90247499999998</v>
+      </c>
+      <c r="C7" s="1">
+        <v>18.302251999999999</v>
+      </c>
+      <c r="D7" s="5">
+        <v>196.60434900000001</v>
+      </c>
+      <c r="E7" s="22">
+        <v>63.919232999999998</v>
+      </c>
+      <c r="F7" s="5">
+        <v>5.6274410000000001</v>
+      </c>
+      <c r="G7" s="24">
+        <v>0.51524099999999995</v>
+      </c>
+      <c r="H7" s="1">
+        <v>15.336581000000001</v>
+      </c>
+      <c r="I7" s="9">
+        <v>642</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>0.06</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="9"/>
+      <c r="B8" s="5">
+        <v>277.058156</v>
+      </c>
+      <c r="C8" s="1">
+        <v>38.440229000000002</v>
+      </c>
+      <c r="D8" s="5">
+        <v>196.624763</v>
+      </c>
+      <c r="E8" s="22">
+        <v>63.850493</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5.6159270000000001</v>
+      </c>
+      <c r="G8" s="24">
+        <v>0.517625</v>
+      </c>
+      <c r="H8" s="1">
+        <v>15.387765</v>
+      </c>
+      <c r="I8" s="9">
+        <v>622</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="9"/>
+      <c r="B9" s="5">
+        <v>392.89157499999999</v>
+      </c>
+      <c r="C9" s="1">
+        <v>22.684142000000001</v>
+      </c>
+      <c r="D9" s="5">
+        <v>196.64531199999999</v>
+      </c>
+      <c r="E9" s="22">
+        <v>63.781230999999998</v>
+      </c>
+      <c r="F9" s="5">
+        <v>5.6043349999999998</v>
+      </c>
+      <c r="G9" s="24">
+        <v>0.52003999999999995</v>
+      </c>
+      <c r="H9" s="1">
+        <v>15.439563</v>
+      </c>
+      <c r="I9" s="9">
+        <v>757</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>0.08</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="9"/>
+      <c r="B10" s="5">
+        <v>912.02342799999997</v>
+      </c>
+      <c r="C10" s="1">
+        <v>35.420658000000003</v>
+      </c>
+      <c r="D10" s="5">
+        <v>196.66597899999999</v>
+      </c>
+      <c r="E10" s="22">
+        <v>63.711413</v>
+      </c>
+      <c r="F10" s="5">
+        <v>5.5926600000000004</v>
+      </c>
+      <c r="G10" s="24">
+        <v>0.52248799999999995</v>
+      </c>
+      <c r="H10" s="1">
+        <v>15.492005000000001</v>
+      </c>
+      <c r="I10" s="9">
+        <v>638</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>0.09</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="9"/>
+      <c r="B11" s="5">
+        <v>793.50692500000002</v>
+      </c>
+      <c r="C11" s="1">
+        <v>13.102698999999999</v>
+      </c>
+      <c r="D11" s="5">
+        <v>196.68677500000001</v>
+      </c>
+      <c r="E11" s="22">
+        <v>63.641033</v>
+      </c>
+      <c r="F11" s="5">
+        <v>5.5809009999999999</v>
+      </c>
+      <c r="G11" s="24">
+        <v>0.52497000000000005</v>
+      </c>
+      <c r="H11" s="1">
+        <v>15.545102999999999</v>
+      </c>
+      <c r="I11" s="9">
+        <v>782</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>0.1</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="9"/>
+      <c r="B12" s="5">
+        <v>593.60388799999998</v>
+      </c>
+      <c r="C12" s="1">
+        <v>11.137857</v>
+      </c>
+      <c r="D12" s="5">
+        <v>196.70769300000001</v>
+      </c>
+      <c r="E12" s="22">
+        <v>63.570087999999998</v>
+      </c>
+      <c r="F12" s="5">
+        <v>5.5690580000000001</v>
+      </c>
+      <c r="G12" s="24">
+        <v>0.52748499999999998</v>
+      </c>
+      <c r="H12" s="1">
+        <v>15.598865</v>
+      </c>
+      <c r="I12" s="9">
+        <v>769</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>0.11</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="9"/>
+      <c r="B13" s="5">
+        <v>688.98251000000005</v>
+      </c>
+      <c r="C13" s="1">
+        <v>30.156495</v>
+      </c>
+      <c r="D13" s="5">
+        <v>196.72875300000001</v>
+      </c>
+      <c r="E13" s="22">
+        <v>63.498570999999998</v>
+      </c>
+      <c r="F13" s="5">
+        <v>5.5571289999999998</v>
+      </c>
+      <c r="G13" s="24">
+        <v>0.53003599999999995</v>
+      </c>
+      <c r="H13" s="1">
+        <v>15.653306000000001</v>
+      </c>
+      <c r="I13" s="9">
+        <v>635</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>0.12</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="9"/>
+      <c r="B14" s="5">
+        <v>598.68377999999996</v>
+      </c>
+      <c r="C14" s="1">
+        <v>48.878653</v>
+      </c>
+      <c r="D14" s="5">
+        <v>196.75017199999999</v>
+      </c>
+      <c r="E14" s="22">
+        <v>63.426439000000002</v>
+      </c>
+      <c r="F14" s="5">
+        <v>5.5451139999999999</v>
+      </c>
+      <c r="G14" s="24">
+        <v>0.53262500000000002</v>
+      </c>
+      <c r="H14" s="1">
+        <v>15.708482999999999</v>
+      </c>
+      <c r="I14" s="9">
+        <v>483</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>0.13</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="9"/>
+      <c r="B15" s="5">
+        <v>270.25691599999999</v>
+      </c>
+      <c r="C15" s="1">
+        <v>42.981206</v>
+      </c>
+      <c r="D15" s="5">
+        <v>196.77125899999999</v>
+      </c>
+      <c r="E15" s="22">
+        <v>63.353734000000003</v>
+      </c>
+      <c r="F15" s="5">
+        <v>5.5330019999999998</v>
+      </c>
+      <c r="G15" s="24">
+        <v>0.535246</v>
+      </c>
+      <c r="H15" s="1">
+        <v>15.764315</v>
+      </c>
+      <c r="I15" s="9">
+        <v>605</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>0.14000000000000001</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="9"/>
+      <c r="B16" s="5">
+        <v>711.98872400000005</v>
+      </c>
+      <c r="C16" s="1">
+        <v>38.665090999999997</v>
+      </c>
+      <c r="D16" s="5">
+        <v>196.79271499999999</v>
+      </c>
+      <c r="E16" s="22">
+        <v>63.280402000000002</v>
+      </c>
+      <c r="F16" s="5">
+        <v>5.5208019999999998</v>
+      </c>
+      <c r="G16" s="24">
+        <v>0.53790800000000005</v>
+      </c>
+      <c r="H16" s="1">
+        <v>15.820909</v>
+      </c>
+      <c r="I16" s="9">
+        <v>638</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>0.15</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="9"/>
+      <c r="B17" s="5">
+        <v>479.558111</v>
+      </c>
+      <c r="C17" s="1">
+        <v>22.452756999999998</v>
+      </c>
+      <c r="D17" s="5">
+        <v>196.81432100000001</v>
+      </c>
+      <c r="E17" s="22">
+        <v>63.206462999999999</v>
+      </c>
+      <c r="F17" s="5">
+        <v>5.5085129999999998</v>
+      </c>
+      <c r="G17" s="24">
+        <v>0.54060699999999995</v>
+      </c>
+      <c r="H17" s="1">
+        <v>15.878239000000001</v>
+      </c>
+      <c r="I17" s="9">
+        <v>642</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>0.16</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="9"/>
+      <c r="B18" s="5">
+        <v>571.34436600000004</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43.574536999999999</v>
+      </c>
+      <c r="D18" s="5">
+        <v>196.83605499999999</v>
+      </c>
+      <c r="E18" s="22">
+        <v>63.131869000000002</v>
+      </c>
+      <c r="F18" s="5">
+        <v>5.4961260000000003</v>
+      </c>
+      <c r="G18" s="24">
+        <v>0.54334700000000002</v>
+      </c>
+      <c r="H18" s="1">
+        <v>15.936349</v>
+      </c>
+      <c r="I18" s="9">
+        <v>604</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>0.17</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="9"/>
+      <c r="B19" s="5">
+        <v>875.96661400000005</v>
+      </c>
+      <c r="C19" s="1">
+        <v>36.829599000000002</v>
+      </c>
+      <c r="D19" s="5">
+        <v>196.85793799999999</v>
+      </c>
+      <c r="E19" s="22">
+        <v>63.056631000000003</v>
+      </c>
+      <c r="F19" s="5">
+        <v>5.4836429999999998</v>
+      </c>
+      <c r="G19" s="24">
+        <v>0.54612700000000003</v>
+      </c>
+      <c r="H19" s="1">
+        <v>15.995239</v>
+      </c>
+      <c r="I19" s="9">
+        <v>651</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>0.18</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="9"/>
+      <c r="B20" s="5">
+        <v>421.04710899999998</v>
+      </c>
+      <c r="C20" s="1">
+        <v>28.660250000000001</v>
+      </c>
+      <c r="D20" s="5">
+        <v>196.879976</v>
+      </c>
+      <c r="E20" s="22">
+        <v>62.980747999999998</v>
+      </c>
+      <c r="F20" s="5">
+        <v>5.4710660000000004</v>
+      </c>
+      <c r="G20" s="24">
+        <v>0.54894799999999999</v>
+      </c>
+      <c r="H20" s="1">
+        <v>16.054922000000001</v>
+      </c>
+      <c r="I20" s="9">
+        <v>629</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>0.19</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="9"/>
+      <c r="B21" s="5">
+        <v>641.657781</v>
+      </c>
+      <c r="C21" s="1">
+        <v>38.832228000000001</v>
+      </c>
+      <c r="D21" s="5">
+        <v>196.902152</v>
+      </c>
+      <c r="E21" s="22">
+        <v>62.904172000000003</v>
+      </c>
+      <c r="F21" s="5">
+        <v>5.4583839999999997</v>
+      </c>
+      <c r="G21" s="24">
+        <v>0.55181199999999997</v>
+      </c>
+      <c r="H21" s="1">
+        <v>16.115441000000001</v>
+      </c>
+      <c r="I21" s="9">
+        <v>624</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>0.2</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="9"/>
+      <c r="B22" s="5">
+        <v>402.50811099999999</v>
+      </c>
+      <c r="C22" s="1">
+        <v>19.042527</v>
+      </c>
+      <c r="D22" s="5">
+        <v>196.924487</v>
+      </c>
+      <c r="E22" s="22">
+        <v>62.826912999999998</v>
+      </c>
+      <c r="F22" s="5">
+        <v>5.4456020000000001</v>
+      </c>
+      <c r="G22" s="24">
+        <v>0.55471999999999999</v>
+      </c>
+      <c r="H22" s="1">
+        <v>16.176801999999999</v>
+      </c>
+      <c r="I22" s="9">
+        <v>768</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>0.21</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="9"/>
+      <c r="B23" s="5">
+        <v>946.02137300000004</v>
+      </c>
+      <c r="C23" s="1">
+        <v>10.832682999999999</v>
+      </c>
+      <c r="D23" s="5">
+        <v>196.94695999999999</v>
+      </c>
+      <c r="E23" s="22">
+        <v>62.748935000000003</v>
+      </c>
+      <c r="F23" s="5">
+        <v>5.4327129999999997</v>
+      </c>
+      <c r="G23" s="24">
+        <v>0.557674</v>
+      </c>
+      <c r="H23" s="1">
+        <v>16.239038000000001</v>
+      </c>
+      <c r="I23" s="9">
+        <v>665</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>0.22</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="9"/>
+      <c r="B24" s="5">
+        <v>957.58503099999996</v>
+      </c>
+      <c r="C24" s="1">
+        <v>40.932108999999997</v>
+      </c>
+      <c r="D24" s="5">
+        <v>196.96824799999999</v>
+      </c>
+      <c r="E24" s="22">
+        <v>62.670332999999999</v>
+      </c>
+      <c r="F24" s="5">
+        <v>5.4196960000000001</v>
+      </c>
+      <c r="G24" s="24">
+        <v>0.56065799999999999</v>
+      </c>
+      <c r="H24" s="1">
+        <v>16.301978999999999</v>
+      </c>
+      <c r="I24" s="9">
+        <v>502</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>0.23</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="9"/>
+      <c r="B25" s="5">
+        <v>891.38490999999999</v>
+      </c>
+      <c r="C25" s="1">
+        <v>48.622447999999999</v>
+      </c>
+      <c r="D25" s="5">
+        <v>196.99232699999999</v>
+      </c>
+      <c r="E25" s="22">
+        <v>62.590885999999998</v>
+      </c>
+      <c r="F25" s="5">
+        <v>5.406625</v>
+      </c>
+      <c r="G25" s="24">
+        <v>0.56371700000000002</v>
+      </c>
+      <c r="H25" s="1">
+        <v>16.366133999999999</v>
+      </c>
+      <c r="I25" s="9">
+        <v>487</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>0.24</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="9"/>
+      <c r="B26" s="5">
+        <v>611.15578300000004</v>
+      </c>
+      <c r="C26" s="1">
+        <v>23.708480999999999</v>
+      </c>
+      <c r="D26" s="5">
+        <v>197.015401</v>
+      </c>
+      <c r="E26" s="22">
+        <v>62.510745</v>
+      </c>
+      <c r="F26" s="5">
+        <v>5.3934199999999999</v>
+      </c>
+      <c r="G26" s="24">
+        <v>0.56681300000000001</v>
+      </c>
+      <c r="H26" s="1">
+        <v>16.431084999999999</v>
+      </c>
+      <c r="I26" s="9">
+        <v>648</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>0.25</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="9"/>
+      <c r="B27" s="5">
+        <v>749.80480299999999</v>
+      </c>
+      <c r="C27" s="1">
+        <v>18.150873000000001</v>
+      </c>
+      <c r="D27" s="5">
+        <v>197.038543</v>
+      </c>
+      <c r="E27" s="22">
+        <v>62.429842000000001</v>
+      </c>
+      <c r="F27" s="5">
+        <v>5.3801009999999998</v>
+      </c>
+      <c r="G27" s="24">
+        <v>0.56995700000000005</v>
+      </c>
+      <c r="H27" s="1">
+        <v>16.496984999999999</v>
+      </c>
+      <c r="I27" s="9">
+        <v>641</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>0.26</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="9"/>
+      <c r="B28" s="5">
+        <v>723.96007599999996</v>
+      </c>
+      <c r="C28" s="1">
+        <v>27.85829</v>
+      </c>
+      <c r="D28" s="5">
+        <v>197.061849</v>
+      </c>
+      <c r="E28" s="22">
+        <v>62.348157999999998</v>
+      </c>
+      <c r="F28" s="5">
+        <v>5.3666660000000004</v>
+      </c>
+      <c r="G28" s="24">
+        <v>0.57315300000000002</v>
+      </c>
+      <c r="H28" s="1">
+        <v>16.563869</v>
+      </c>
+      <c r="I28" s="9">
+        <v>639</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>0.27</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="9"/>
+      <c r="B29" s="5">
+        <v>455.96094900000003</v>
+      </c>
+      <c r="C29" s="1">
+        <v>21.086203000000001</v>
+      </c>
+      <c r="D29" s="5">
+        <v>197.085317</v>
+      </c>
+      <c r="E29" s="22">
+        <v>62.265649000000003</v>
+      </c>
+      <c r="F29" s="5">
+        <v>5.3531079999999998</v>
+      </c>
+      <c r="G29" s="24">
+        <v>0.576403</v>
+      </c>
+      <c r="H29" s="1">
+        <v>16.631782999999999</v>
+      </c>
+      <c r="I29" s="9">
+        <v>659</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="9"/>
+      <c r="B30" s="5">
+        <v>806.99087799999995</v>
+      </c>
+      <c r="C30" s="1">
+        <v>20.066324000000002</v>
+      </c>
+      <c r="D30" s="5">
+        <v>197.10897499999999</v>
+      </c>
+      <c r="E30" s="22">
+        <v>62.182352999999999</v>
+      </c>
+      <c r="F30" s="5">
+        <v>5.3394370000000002</v>
+      </c>
+      <c r="G30" s="24">
+        <v>0.57970699999999997</v>
+      </c>
+      <c r="H30" s="1">
+        <v>16.700714999999999</v>
+      </c>
+      <c r="I30" s="9">
+        <v>660</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="9"/>
+      <c r="B31" s="5">
+        <v>690.34256100000005</v>
+      </c>
+      <c r="C31" s="1">
+        <v>36.694541999999998</v>
+      </c>
+      <c r="D31" s="5">
+        <v>197.13282100000001</v>
+      </c>
+      <c r="E31" s="22">
+        <v>62.098247000000001</v>
+      </c>
+      <c r="F31" s="5">
+        <v>5.325647</v>
+      </c>
+      <c r="G31" s="24">
+        <v>0.58306500000000006</v>
+      </c>
+      <c r="H31" s="1">
+        <v>16.770693000000001</v>
+      </c>
+      <c r="I31" s="9">
+        <v>633</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>0.3</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="9"/>
+      <c r="B32" s="5">
+        <v>898.48886300000004</v>
+      </c>
+      <c r="C32" s="1">
+        <v>28.949954999999999</v>
+      </c>
+      <c r="D32" s="5">
+        <v>197.15684300000001</v>
+      </c>
+      <c r="E32" s="22">
+        <v>62.013275</v>
+      </c>
+      <c r="F32" s="5">
+        <v>5.3117289999999997</v>
+      </c>
+      <c r="G32" s="24">
+        <v>0.58648199999999995</v>
+      </c>
+      <c r="H32" s="1">
+        <v>16.841778999999999</v>
+      </c>
+      <c r="I32" s="9">
+        <v>651</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>0.31</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="9"/>
+      <c r="B33" s="5">
+        <v>270.68838699999998</v>
+      </c>
+      <c r="C33" s="1">
+        <v>11.68534</v>
+      </c>
+      <c r="D33" s="5">
+        <v>197.18105299999999</v>
+      </c>
+      <c r="E33" s="22">
+        <v>61.927436</v>
+      </c>
+      <c r="F33" s="5">
+        <v>5.2976850000000004</v>
+      </c>
+      <c r="G33" s="24">
+        <v>0.58995799999999998</v>
+      </c>
+      <c r="H33" s="1">
+        <v>16.913986999999999</v>
+      </c>
+      <c r="I33" s="9">
+        <v>919</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>0.32</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="9"/>
+      <c r="B34" s="5">
+        <v>464.83945599999998</v>
+      </c>
+      <c r="C34" s="1">
+        <v>42.569324000000002</v>
+      </c>
+      <c r="D34" s="5">
+        <v>197.20579799999999</v>
+      </c>
+      <c r="E34" s="22">
+        <v>61.840684000000003</v>
+      </c>
+      <c r="F34" s="5">
+        <v>5.2835159999999997</v>
+      </c>
+      <c r="G34" s="24">
+        <v>0.59349799999999997</v>
+      </c>
+      <c r="H34" s="1">
+        <v>16.987400000000001</v>
+      </c>
+      <c r="I34" s="9">
+        <v>497</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>0.33</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="9"/>
+      <c r="B35" s="5">
+        <v>715.72703999999999</v>
+      </c>
+      <c r="C35" s="1">
+        <v>46.671768999999998</v>
+      </c>
+      <c r="D35" s="5">
+        <v>197.22922</v>
+      </c>
+      <c r="E35" s="22">
+        <v>61.753095999999999</v>
+      </c>
+      <c r="F35" s="5">
+        <v>5.2691850000000002</v>
+      </c>
+      <c r="G35" s="24">
+        <v>0.59708499999999998</v>
+      </c>
+      <c r="H35" s="1">
+        <v>17.061812</v>
+      </c>
+      <c r="I35" s="9">
+        <v>475</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>0.34</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="9"/>
+      <c r="B36" s="5">
+        <v>907.17598199999998</v>
+      </c>
+      <c r="C36" s="1">
+        <v>27.557407999999999</v>
+      </c>
+      <c r="D36" s="5">
+        <v>197.25484800000001</v>
+      </c>
+      <c r="E36" s="22">
+        <v>61.664503000000003</v>
+      </c>
+      <c r="F36" s="5">
+        <v>5.2547600000000001</v>
+      </c>
+      <c r="G36" s="24">
+        <v>0.60075800000000001</v>
+      </c>
+      <c r="H36" s="1">
+        <v>17.137682000000002</v>
+      </c>
+      <c r="I36" s="9">
+        <v>642</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>0.35000000000000003</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="9"/>
+      <c r="B37" s="5">
+        <v>553.93342399999995</v>
+      </c>
+      <c r="C37" s="1">
+        <v>49.939728000000002</v>
+      </c>
+      <c r="D37" s="5">
+        <v>197.28061500000001</v>
+      </c>
+      <c r="E37" s="22">
+        <v>61.574953999999998</v>
+      </c>
+      <c r="F37" s="5">
+        <v>5.2401939999999998</v>
+      </c>
+      <c r="G37" s="24">
+        <v>0.60449699999999995</v>
+      </c>
+      <c r="H37" s="1">
+        <v>17.21481</v>
+      </c>
+      <c r="I37" s="9">
+        <v>469</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>0.36</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="9"/>
+      <c r="B38" s="5">
+        <v>493.86576500000001</v>
+      </c>
+      <c r="C38" s="1">
+        <v>11.513623000000001</v>
+      </c>
+      <c r="D38" s="5">
+        <v>197.305058</v>
+      </c>
+      <c r="E38" s="22">
+        <v>61.484482</v>
+      </c>
+      <c r="F38" s="5">
+        <v>5.225454</v>
+      </c>
+      <c r="G38" s="24">
+        <v>0.60828899999999997</v>
+      </c>
+      <c r="H38" s="1">
+        <v>17.293057000000001</v>
+      </c>
+      <c r="I38" s="9">
+        <v>781</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>0.37</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="9"/>
+      <c r="B39" s="5">
+        <v>314.86278700000003</v>
+      </c>
+      <c r="C39" s="1">
+        <v>16.802222</v>
+      </c>
+      <c r="D39" s="5">
+        <v>197.330476</v>
+      </c>
+      <c r="E39" s="22">
+        <v>61.392985000000003</v>
+      </c>
+      <c r="F39" s="5">
+        <v>5.2105839999999999</v>
+      </c>
+      <c r="G39" s="24">
+        <v>0.61216000000000004</v>
+      </c>
+      <c r="H39" s="1">
+        <v>17.372727999999999</v>
+      </c>
+      <c r="I39" s="9">
+        <v>775</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>0.38</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="9"/>
+      <c r="B40" s="5">
+        <v>895.59969599999999</v>
+      </c>
+      <c r="C40" s="1">
+        <v>15.355828000000001</v>
+      </c>
+      <c r="D40" s="5">
+        <v>197.35612499999999</v>
+      </c>
+      <c r="E40" s="22">
+        <v>61.300469999999997</v>
+      </c>
+      <c r="F40" s="5">
+        <v>5.1955669999999996</v>
+      </c>
+      <c r="G40" s="24">
+        <v>0.61610399999999998</v>
+      </c>
+      <c r="H40" s="1">
+        <v>17.453772000000001</v>
+      </c>
+      <c r="I40" s="9">
+        <v>651</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>0.39</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="9"/>
+      <c r="B41" s="5">
+        <v>413.078011</v>
+      </c>
+      <c r="C41" s="1">
+        <v>25.089386000000001</v>
+      </c>
+      <c r="D41" s="5">
+        <v>197.38198600000001</v>
+      </c>
+      <c r="E41" s="22">
+        <v>61.206885999999997</v>
+      </c>
+      <c r="F41" s="5">
+        <v>5.1803939999999997</v>
+      </c>
+      <c r="G41" s="24">
+        <v>0.62012500000000004</v>
+      </c>
+      <c r="H41" s="1">
+        <v>17.536252000000001</v>
+      </c>
+      <c r="I41" s="9">
+        <v>633</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>0.4</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="9"/>
+      <c r="B42" s="5">
+        <v>530.23888499999998</v>
+      </c>
+      <c r="C42" s="1">
+        <v>14.558804</v>
+      </c>
+      <c r="D42" s="5">
+        <v>197.408072</v>
+      </c>
+      <c r="E42" s="22">
+        <v>61.112223999999998</v>
+      </c>
+      <c r="F42" s="5">
+        <v>5.1650650000000002</v>
+      </c>
+      <c r="G42" s="24">
+        <v>0.62422299999999997</v>
+      </c>
+      <c r="H42" s="1">
+        <v>17.620196</v>
+      </c>
+      <c r="I42" s="9">
+        <v>758</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>0.41000000000000003</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="9"/>
+      <c r="B43" s="5">
+        <v>603.65393400000005</v>
+      </c>
+      <c r="C43" s="1">
+        <v>49.986933000000001</v>
+      </c>
+      <c r="D43" s="5">
+        <v>197.43506099999999</v>
+      </c>
+      <c r="E43" s="22">
+        <v>61.016441</v>
+      </c>
+      <c r="F43" s="5">
+        <v>5.149591</v>
+      </c>
+      <c r="G43" s="24">
+        <v>0.62841000000000002</v>
+      </c>
+      <c r="H43" s="1">
+        <v>17.705727</v>
+      </c>
+      <c r="I43" s="9">
+        <v>474</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>0.42</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="9"/>
+      <c r="B44" s="5">
+        <v>253.38781900000001</v>
+      </c>
+      <c r="C44" s="1">
+        <v>15.579147000000001</v>
+      </c>
+      <c r="D44" s="5">
+        <v>197.46096</v>
+      </c>
+      <c r="E44" s="22">
+        <v>60.919556999999998</v>
+      </c>
+      <c r="F44" s="5">
+        <v>5.1339240000000004</v>
+      </c>
+      <c r="G44" s="24">
+        <v>0.63266599999999995</v>
+      </c>
+      <c r="H44" s="1">
+        <v>17.792670000000001</v>
+      </c>
+      <c r="I44" s="9">
+        <v>901</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>0.43</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="9"/>
+      <c r="B45" s="5">
+        <v>476.84151200000002</v>
+      </c>
+      <c r="C45" s="1">
+        <v>24.331299000000001</v>
+      </c>
+      <c r="D45" s="5">
+        <v>197.487762</v>
+      </c>
+      <c r="E45" s="22">
+        <v>60.821475999999997</v>
+      </c>
+      <c r="F45" s="5">
+        <v>5.1181010000000002</v>
+      </c>
+      <c r="G45" s="24">
+        <v>0.63701600000000003</v>
+      </c>
+      <c r="H45" s="1">
+        <v>17.881314</v>
+      </c>
+      <c r="I45" s="9">
+        <v>649</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>0.44</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="9"/>
+      <c r="B46" s="5">
+        <v>584.62049000000002</v>
+      </c>
+      <c r="C46" s="1">
+        <v>20.541530999999999</v>
+      </c>
+      <c r="D46" s="5">
+        <v>197.51482999999999</v>
+      </c>
+      <c r="E46" s="22">
+        <v>60.722228000000001</v>
+      </c>
+      <c r="F46" s="5">
+        <v>5.1021099999999997</v>
+      </c>
+      <c r="G46" s="24">
+        <v>0.641455</v>
+      </c>
+      <c r="H46" s="1">
+        <v>17.971599000000001</v>
+      </c>
+      <c r="I46" s="9">
+        <v>645</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>0.45</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="9"/>
+      <c r="B47" s="5">
+        <v>753.94581400000004</v>
+      </c>
+      <c r="C47" s="1">
+        <v>32.736682000000002</v>
+      </c>
+      <c r="D47" s="5">
+        <v>197.54213999999999</v>
+      </c>
+      <c r="E47" s="22">
+        <v>60.621713</v>
+      </c>
+      <c r="F47" s="5">
+        <v>5.0859360000000002</v>
+      </c>
+      <c r="G47" s="24">
+        <v>0.64598699999999998</v>
+      </c>
+      <c r="H47" s="1">
+        <v>18.063638999999998</v>
+      </c>
+      <c r="I47" s="9">
+        <v>632</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>0.46</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="9"/>
+      <c r="B48" s="5">
+        <v>866.442274</v>
+      </c>
+      <c r="C48" s="1">
+        <v>30.283438</v>
+      </c>
+      <c r="D48" s="5">
+        <v>197.56971899999999</v>
+      </c>
+      <c r="E48" s="22">
+        <v>60.519945</v>
+      </c>
+      <c r="F48" s="5">
+        <v>5.0695819999999996</v>
+      </c>
+      <c r="G48" s="24">
+        <v>0.65061599999999997</v>
+      </c>
+      <c r="H48" s="1">
+        <v>18.157451999999999</v>
+      </c>
+      <c r="I48" s="9">
+        <v>756</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <v>0.47000000000000003</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="9"/>
+      <c r="B49" s="5">
+        <v>873.51429900000005</v>
+      </c>
+      <c r="C49" s="1">
+        <v>29.590523000000001</v>
+      </c>
+      <c r="D49" s="5">
+        <v>197.59756899999999</v>
+      </c>
+      <c r="E49" s="22">
+        <v>60.416874</v>
+      </c>
+      <c r="F49" s="5">
+        <v>5.0530410000000003</v>
+      </c>
+      <c r="G49" s="24">
+        <v>0.65534400000000004</v>
+      </c>
+      <c r="H49" s="1">
+        <v>18.253114</v>
+      </c>
+      <c r="I49" s="9">
+        <v>646</v>
+      </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
         <v>0.48</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="9"/>
+      <c r="B50" s="5">
+        <v>380.74088999999998</v>
+      </c>
+      <c r="C50" s="1">
+        <v>48.850231000000001</v>
+      </c>
+      <c r="D50" s="5">
+        <v>197.62564599999999</v>
+      </c>
+      <c r="E50" s="22">
+        <v>60.312451000000003</v>
+      </c>
+      <c r="F50" s="5">
+        <v>5.0363049999999996</v>
+      </c>
+      <c r="G50" s="24">
+        <v>0.66017599999999999</v>
+      </c>
+      <c r="H50" s="1">
+        <v>18.350693</v>
+      </c>
+      <c r="I50" s="9">
+        <v>470</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <v>0.49</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="9"/>
+      <c r="B51" s="5">
+        <v>245.71668399999999</v>
+      </c>
+      <c r="C51" s="1">
+        <v>32.265892999999998</v>
+      </c>
+      <c r="D51" s="5">
+        <v>197.65409399999999</v>
+      </c>
+      <c r="E51" s="22">
+        <v>60.206636000000003</v>
+      </c>
+      <c r="F51" s="5">
+        <v>5.0193709999999996</v>
+      </c>
+      <c r="G51" s="24">
+        <v>0.66511600000000004</v>
+      </c>
+      <c r="H51" s="1">
+        <v>18.450275000000001</v>
+      </c>
+      <c r="I51" s="9">
+        <v>641</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>0.5</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="9"/>
+      <c r="B52" s="5">
+        <v>914.87975300000005</v>
+      </c>
+      <c r="C52" s="1">
+        <v>31.291238</v>
+      </c>
+      <c r="D52" s="5">
+        <v>197.68280799999999</v>
+      </c>
+      <c r="E52" s="22">
+        <v>60.099420000000002</v>
+      </c>
+      <c r="F52" s="5">
+        <v>5.0022359999999999</v>
+      </c>
+      <c r="G52" s="24">
+        <v>0.67016699999999996</v>
+      </c>
+      <c r="H52" s="1">
+        <v>18.55189</v>
+      </c>
+      <c r="I52" s="9">
+        <v>640</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>0.51</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="9"/>
+      <c r="B53" s="5">
+        <v>647.30332899999996</v>
+      </c>
+      <c r="C53" s="1">
+        <v>23.351749000000002</v>
+      </c>
+      <c r="D53" s="5">
+        <v>197.71181200000001</v>
+      </c>
+      <c r="E53" s="22">
+        <v>59.990724999999998</v>
+      </c>
+      <c r="F53" s="5">
+        <v>4.98489</v>
+      </c>
+      <c r="G53" s="24">
+        <v>0.67533500000000002</v>
+      </c>
+      <c r="H53" s="1">
+        <v>18.655650000000001</v>
+      </c>
+      <c r="I53" s="9">
+        <v>644</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <v>0.52</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="9"/>
+      <c r="B54" s="5">
+        <v>396.530509</v>
+      </c>
+      <c r="C54" s="1">
+        <v>27.025511000000002</v>
+      </c>
+      <c r="D54" s="5">
+        <v>197.74112299999999</v>
+      </c>
+      <c r="E54" s="22">
+        <v>59.880509000000004</v>
+      </c>
+      <c r="F54" s="5">
+        <v>4.9673259999999999</v>
+      </c>
+      <c r="G54" s="24">
+        <v>0.68062299999999998</v>
+      </c>
+      <c r="H54" s="1">
+        <v>18.761633</v>
+      </c>
+      <c r="I54" s="9">
+        <v>632</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>0.53</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="9"/>
+      <c r="B55" s="5">
+        <v>470.381576</v>
+      </c>
+      <c r="C55" s="1">
+        <v>39.896237999999997</v>
+      </c>
+      <c r="D55" s="5">
+        <v>197.771353</v>
+      </c>
+      <c r="E55" s="22">
+        <v>59.768689999999999</v>
+      </c>
+      <c r="F55" s="5">
+        <v>4.9495490000000002</v>
+      </c>
+      <c r="G55" s="24">
+        <v>0.68604500000000002</v>
+      </c>
+      <c r="H55" s="1">
+        <v>18.870016</v>
+      </c>
+      <c r="I55" s="9">
+        <v>499</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
         <v>0.54</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="9"/>
+      <c r="B56" s="5">
+        <v>605.44617900000003</v>
+      </c>
+      <c r="C56" s="1">
+        <v>26.080089999999998</v>
+      </c>
+      <c r="D56" s="5">
+        <v>197.80070900000001</v>
+      </c>
+      <c r="E56" s="22">
+        <v>59.655341</v>
+      </c>
+      <c r="F56" s="5">
+        <v>4.9315249999999997</v>
+      </c>
+      <c r="G56" s="24">
+        <v>0.69158200000000003</v>
+      </c>
+      <c r="H56" s="1">
+        <v>18.980599999999999</v>
+      </c>
+      <c r="I56" s="9">
+        <v>640</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="9"/>
+      <c r="B57" s="5">
+        <v>448.95053799999999</v>
+      </c>
+      <c r="C57" s="1">
+        <v>24.555751999999998</v>
+      </c>
+      <c r="D57" s="5">
+        <v>197.83100099999999</v>
+      </c>
+      <c r="E57" s="22">
+        <v>59.540281999999998</v>
+      </c>
+      <c r="F57" s="5">
+        <v>4.9132730000000002</v>
+      </c>
+      <c r="G57" s="24">
+        <v>0.69726399999999999</v>
+      </c>
+      <c r="H57" s="1">
+        <v>19.093775000000001</v>
+      </c>
+      <c r="I57" s="9">
+        <v>641</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>0.56000000000000005</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="9"/>
+      <c r="B58" s="5">
+        <v>821.15774399999998</v>
+      </c>
+      <c r="C58" s="1">
+        <v>43.499693000000001</v>
+      </c>
+      <c r="D58" s="5">
+        <v>197.86229499999999</v>
+      </c>
+      <c r="E58" s="22">
+        <v>59.423490000000001</v>
+      </c>
+      <c r="F58" s="5">
+        <v>4.8947900000000004</v>
+      </c>
+      <c r="G58" s="24">
+        <v>0.70309500000000003</v>
+      </c>
+      <c r="H58" s="1">
+        <v>19.209614999999999</v>
+      </c>
+      <c r="I58" s="9">
+        <v>490</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>0.57000000000000006</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="9"/>
+      <c r="B59" s="5">
+        <v>250.36944500000001</v>
+      </c>
+      <c r="C59" s="1">
+        <v>47.219799999999999</v>
+      </c>
+      <c r="D59" s="5">
+        <v>197.89264399999999</v>
+      </c>
+      <c r="E59" s="22">
+        <v>59.304944999999996</v>
+      </c>
+      <c r="F59" s="5">
+        <v>4.8760279999999998</v>
+      </c>
+      <c r="G59" s="24">
+        <v>0.70906000000000002</v>
+      </c>
+      <c r="H59" s="1">
+        <v>19.328005000000001</v>
+      </c>
+      <c r="I59" s="9">
+        <v>571</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>0.57999999999999996</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="24"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="9"/>
+      <c r="B60" s="5">
+        <v>557.09866799999998</v>
+      </c>
+      <c r="C60" s="1">
+        <v>13.195328999999999</v>
+      </c>
+      <c r="D60" s="5">
+        <v>197.92400699999999</v>
+      </c>
+      <c r="E60" s="22">
+        <v>59.184530000000002</v>
+      </c>
+      <c r="F60" s="5">
+        <v>4.8570169999999999</v>
+      </c>
+      <c r="G60" s="24">
+        <v>0.71518800000000005</v>
+      </c>
+      <c r="H60" s="1">
+        <v>19.449300000000001</v>
+      </c>
+      <c r="I60" s="9">
+        <v>656</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>0.59</v>
       </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="24"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="9"/>
+      <c r="B61" s="5">
+        <v>797.14235399999995</v>
+      </c>
+      <c r="C61" s="1">
+        <v>40.111662000000003</v>
+      </c>
+      <c r="D61" s="5">
+        <v>197.95596499999999</v>
+      </c>
+      <c r="E61" s="22">
+        <v>59.062206000000003</v>
+      </c>
+      <c r="F61" s="5">
+        <v>4.8377410000000003</v>
+      </c>
+      <c r="G61" s="24">
+        <v>0.72148100000000004</v>
+      </c>
+      <c r="H61" s="1">
+        <v>19.573554999999999</v>
+      </c>
+      <c r="I61" s="9">
+        <v>497</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>0.6</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="22"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="24"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="9"/>
+      <c r="B62" s="5">
+        <v>664.08344399999999</v>
+      </c>
+      <c r="C62" s="1">
+        <v>31.929891000000001</v>
+      </c>
+      <c r="D62" s="5">
+        <v>197.98888299999999</v>
+      </c>
+      <c r="E62" s="22">
+        <v>58.937848000000002</v>
+      </c>
+      <c r="F62" s="5">
+        <v>4.8181919999999998</v>
+      </c>
+      <c r="G62" s="24">
+        <v>0.72795200000000004</v>
+      </c>
+      <c r="H62" s="1">
+        <v>19.700991999999999</v>
+      </c>
+      <c r="I62" s="9">
+        <v>512</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>0.61</v>
       </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="24"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="9"/>
+      <c r="B63" s="5">
+        <v>701.93898200000001</v>
+      </c>
+      <c r="C63" s="1">
+        <v>49.185071000000001</v>
+      </c>
+      <c r="D63" s="5">
+        <v>198.020186</v>
+      </c>
+      <c r="E63" s="22">
+        <v>58.811554000000001</v>
+      </c>
+      <c r="F63" s="5">
+        <v>4.7983229999999999</v>
+      </c>
+      <c r="G63" s="24">
+        <v>0.73457399999999995</v>
+      </c>
+      <c r="H63" s="1">
+        <v>19.831319000000001</v>
+      </c>
+      <c r="I63" s="9">
+        <v>462</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>0.62</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="24"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="9"/>
+      <c r="B64" s="5">
+        <v>715.08117600000003</v>
+      </c>
+      <c r="C64" s="1">
+        <v>30.164197000000001</v>
+      </c>
+      <c r="D64" s="5">
+        <v>198.053416</v>
+      </c>
+      <c r="E64" s="22">
+        <v>58.683056999999998</v>
+      </c>
+      <c r="F64" s="5">
+        <v>4.7781799999999999</v>
+      </c>
+      <c r="G64" s="24">
+        <v>0.74140200000000001</v>
+      </c>
+      <c r="H64" s="1">
+        <v>19.965226999999999</v>
+      </c>
+      <c r="I64" s="9">
+        <v>632</v>
+      </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
         <v>0.63</v>
       </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="22"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="24"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="9"/>
+      <c r="B65" s="5">
+        <v>367.00876799999998</v>
+      </c>
+      <c r="C65" s="1">
+        <v>48.144734</v>
+      </c>
+      <c r="D65" s="5">
+        <v>198.08703</v>
+      </c>
+      <c r="E65" s="22">
+        <v>58.552329999999998</v>
+      </c>
+      <c r="F65" s="5">
+        <v>4.7577230000000004</v>
+      </c>
+      <c r="G65" s="24">
+        <v>0.74842600000000004</v>
+      </c>
+      <c r="H65" s="1">
+        <v>20.102663</v>
+      </c>
+      <c r="I65" s="9">
+        <v>465</v>
+      </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="7">
         <v>0.64</v>
       </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="22"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="24"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="9"/>
+      <c r="B66" s="5">
+        <v>223.00351000000001</v>
+      </c>
+      <c r="C66" s="1">
+        <v>13.374826000000001</v>
+      </c>
+      <c r="D66" s="5">
+        <v>198.12067300000001</v>
+      </c>
+      <c r="E66" s="22">
+        <v>58.419325999999998</v>
+      </c>
+      <c r="F66" s="5">
+        <v>4.7369370000000002</v>
+      </c>
+      <c r="G66" s="24">
+        <v>0.75565000000000004</v>
+      </c>
+      <c r="H66" s="1">
+        <v>20.243717</v>
+      </c>
+      <c r="I66" s="9">
+        <v>943</v>
+      </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="7">
         <v>0.65</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="24"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="9"/>
+      <c r="B67" s="5">
+        <v>441.40687100000002</v>
+      </c>
+      <c r="C67" s="1">
+        <v>28.489249000000001</v>
+      </c>
+      <c r="D67" s="5">
+        <v>198.15499500000001</v>
+      </c>
+      <c r="E67" s="22">
+        <v>58.283911000000003</v>
+      </c>
+      <c r="F67" s="5">
+        <v>4.7158189999999998</v>
+      </c>
+      <c r="G67" s="24">
+        <v>0.76309400000000005</v>
+      </c>
+      <c r="H67" s="1">
+        <v>20.388677999999999</v>
+      </c>
+      <c r="I67" s="9">
+        <v>622</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="7">
         <v>0.66</v>
       </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="24"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="9"/>
+      <c r="B68" s="5">
+        <v>491.85135700000001</v>
+      </c>
+      <c r="C68" s="1">
+        <v>34.880085999999999</v>
+      </c>
+      <c r="D68" s="5">
+        <v>198.18979899999999</v>
+      </c>
+      <c r="E68" s="22">
+        <v>58.145989</v>
+      </c>
+      <c r="F68" s="5">
+        <v>4.6943510000000002</v>
+      </c>
+      <c r="G68" s="24">
+        <v>0.77076599999999995</v>
+      </c>
+      <c r="H68" s="1">
+        <v>20.537714999999999</v>
+      </c>
+      <c r="I68" s="9">
+        <v>625</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="7">
         <v>0.67</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="9"/>
+      <c r="B69" s="5">
+        <v>690.06713500000001</v>
+      </c>
+      <c r="C69" s="1">
+        <v>27.729022000000001</v>
+      </c>
+      <c r="D69" s="5">
+        <v>198.22511</v>
+      </c>
+      <c r="E69" s="22">
+        <v>58.005471999999997</v>
+      </c>
+      <c r="F69" s="5">
+        <v>4.6725219999999998</v>
+      </c>
+      <c r="G69" s="24">
+        <v>0.77867799999999998</v>
+      </c>
+      <c r="H69" s="1">
+        <v>20.691019000000001</v>
+      </c>
+      <c r="I69" s="9">
+        <v>635</v>
+      </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="7">
         <v>0.68</v>
       </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="22"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="9"/>
+      <c r="B70" s="5">
+        <v>310.796943</v>
+      </c>
+      <c r="C70" s="1">
+        <v>21.083497999999999</v>
+      </c>
+      <c r="D70" s="5">
+        <v>198.260929</v>
+      </c>
+      <c r="E70" s="22">
+        <v>57.862200000000001</v>
+      </c>
+      <c r="F70" s="5">
+        <v>4.6503079999999999</v>
+      </c>
+      <c r="G70" s="24">
+        <v>0.78684500000000002</v>
+      </c>
+      <c r="H70" s="1">
+        <v>20.848863999999999</v>
+      </c>
+      <c r="I70" s="9">
+        <v>639</v>
+      </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="7">
         <v>0.69000000000000006</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="9"/>
+      <c r="B71" s="5">
+        <v>391.09461299999998</v>
+      </c>
+      <c r="C71" s="1">
+        <v>36.384667999999998</v>
+      </c>
+      <c r="D71" s="5">
+        <v>198.29779199999999</v>
+      </c>
+      <c r="E71" s="22">
+        <v>57.716076000000001</v>
+      </c>
+      <c r="F71" s="5">
+        <v>4.6277109999999997</v>
+      </c>
+      <c r="G71" s="24">
+        <v>0.79528699999999997</v>
+      </c>
+      <c r="H71" s="1">
+        <v>21.011524999999999</v>
+      </c>
+      <c r="I71" s="9">
+        <v>494</v>
+      </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="7">
         <v>0.70000000000000007</v>
       </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="24"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="9"/>
+      <c r="B72" s="5">
+        <v>796.910257</v>
+      </c>
+      <c r="C72" s="1">
+        <v>12.747762</v>
+      </c>
+      <c r="D72" s="5">
+        <v>198.33425399999999</v>
+      </c>
+      <c r="E72" s="22">
+        <v>57.567042000000001</v>
+      </c>
+      <c r="F72" s="5">
+        <v>4.6046889999999996</v>
+      </c>
+      <c r="G72" s="24">
+        <v>0.80399799999999999</v>
+      </c>
+      <c r="H72" s="1">
+        <v>21.179030999999998</v>
+      </c>
+      <c r="I72" s="9">
+        <v>668</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="7">
         <v>0.71</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="24"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="9"/>
+      <c r="B73" s="5">
+        <v>775.85152200000005</v>
+      </c>
+      <c r="C73" s="1">
+        <v>48.282071000000002</v>
+      </c>
+      <c r="D73" s="5">
+        <v>198.370439</v>
+      </c>
+      <c r="E73" s="22">
+        <v>57.414898999999998</v>
+      </c>
+      <c r="F73" s="5">
+        <v>4.5812169999999997</v>
+      </c>
+      <c r="G73" s="24">
+        <v>0.81299900000000003</v>
+      </c>
+      <c r="H73" s="1">
+        <v>21.351738000000001</v>
+      </c>
+      <c r="I73" s="9">
+        <v>462</v>
+      </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="7">
         <v>0.72</v>
       </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="22"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="24"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="9"/>
+      <c r="B74" s="5">
+        <v>208.09306000000001</v>
+      </c>
+      <c r="C74" s="1">
+        <v>19.393739</v>
+      </c>
+      <c r="D74" s="5">
+        <v>198.40994900000001</v>
+      </c>
+      <c r="E74" s="22">
+        <v>57.259430999999999</v>
+      </c>
+      <c r="F74" s="5">
+        <v>4.5573490000000003</v>
+      </c>
+      <c r="G74" s="24">
+        <v>0.82235599999999998</v>
+      </c>
+      <c r="H74" s="1">
+        <v>21.530418000000001</v>
+      </c>
+      <c r="I74" s="9">
+        <v>916</v>
+      </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="7">
         <v>0.73</v>
       </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="24"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="9"/>
+      <c r="B75" s="5">
+        <v>257.38846899999999</v>
+      </c>
+      <c r="C75" s="1">
+        <v>26.676677999999999</v>
+      </c>
+      <c r="D75" s="5">
+        <v>198.448735</v>
+      </c>
+      <c r="E75" s="22">
+        <v>57.100534000000003</v>
+      </c>
+      <c r="F75" s="5">
+        <v>4.5329759999999997</v>
+      </c>
+      <c r="G75" s="24">
+        <v>0.832036</v>
+      </c>
+      <c r="H75" s="1">
+        <v>21.714904000000001</v>
+      </c>
+      <c r="I75" s="9">
+        <v>632</v>
+      </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="7">
         <v>0.74</v>
       </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="22"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="24"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="9"/>
+      <c r="B76" s="5">
+        <v>656.30047300000001</v>
+      </c>
+      <c r="C76" s="1">
+        <v>22.935348999999999</v>
+      </c>
+      <c r="D76" s="5">
+        <v>198.48822000000001</v>
+      </c>
+      <c r="E76" s="22">
+        <v>56.938057000000001</v>
+      </c>
+      <c r="F76" s="5">
+        <v>4.5081129999999998</v>
+      </c>
+      <c r="G76" s="24">
+        <v>0.84207600000000005</v>
+      </c>
+      <c r="H76" s="1">
+        <v>21.905688000000001</v>
+      </c>
+      <c r="I76" s="9">
+        <v>775</v>
+      </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="7">
         <v>0.75</v>
       </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="22"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="24"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="9"/>
+      <c r="B77" s="5">
+        <v>885.70393000000001</v>
+      </c>
+      <c r="C77" s="1">
+        <v>19.479932000000002</v>
+      </c>
+      <c r="D77" s="5">
+        <v>198.52839700000001</v>
+      </c>
+      <c r="E77" s="22">
+        <v>56.771749</v>
+      </c>
+      <c r="F77" s="5">
+        <v>4.482723</v>
+      </c>
+      <c r="G77" s="24">
+        <v>0.85250400000000004</v>
+      </c>
+      <c r="H77" s="1">
+        <v>22.103238000000001</v>
+      </c>
+      <c r="I77" s="9">
+        <v>640</v>
+      </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="7">
         <v>0.76</v>
       </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="22"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="24"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="9"/>
+      <c r="B78" s="5">
+        <v>425.921876</v>
+      </c>
+      <c r="C78" s="1">
+        <v>43.768225000000001</v>
+      </c>
+      <c r="D78" s="5">
+        <v>198.56877700000001</v>
+      </c>
+      <c r="E78" s="22">
+        <v>56.601491000000003</v>
+      </c>
+      <c r="F78" s="5">
+        <v>4.4567819999999996</v>
+      </c>
+      <c r="G78" s="24">
+        <v>0.86333400000000005</v>
+      </c>
+      <c r="H78" s="1">
+        <v>22.307836000000002</v>
+      </c>
+      <c r="I78" s="9">
+        <v>462</v>
+      </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="7">
         <v>0.77</v>
       </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="22"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="9"/>
+      <c r="B79" s="5">
+        <v>256.39101499999998</v>
+      </c>
+      <c r="C79" s="1">
+        <v>21.954626000000001</v>
+      </c>
+      <c r="D79" s="5">
+        <v>198.61103800000001</v>
+      </c>
+      <c r="E79" s="22">
+        <v>56.426935999999998</v>
+      </c>
+      <c r="F79" s="5">
+        <v>4.4302789999999996</v>
+      </c>
+      <c r="G79" s="24">
+        <v>0.87462499999999999</v>
+      </c>
+      <c r="H79" s="1">
+        <v>22.520295999999998</v>
+      </c>
+      <c r="I79" s="9">
+        <v>636</v>
+      </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="7">
         <v>0.78</v>
       </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="24"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="9"/>
+      <c r="B80" s="5">
+        <v>268.06411300000002</v>
+      </c>
+      <c r="C80" s="1">
+        <v>16.810783000000001</v>
+      </c>
+      <c r="D80" s="5">
+        <v>198.65355299999999</v>
+      </c>
+      <c r="E80" s="22">
+        <v>56.247897000000002</v>
+      </c>
+      <c r="F80" s="5">
+        <v>4.4031520000000004</v>
+      </c>
+      <c r="G80" s="24">
+        <v>0.88638300000000003</v>
+      </c>
+      <c r="H80" s="1">
+        <v>22.740895999999999</v>
+      </c>
+      <c r="I80" s="9">
+        <v>769</v>
+      </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="7">
         <v>0.79</v>
       </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="22"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="24"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="9"/>
+      <c r="B81" s="5">
+        <v>740.431738</v>
+      </c>
+      <c r="C81" s="1">
+        <v>34.143400999999997</v>
+      </c>
+      <c r="D81" s="5">
+        <v>198.69631999999999</v>
+      </c>
+      <c r="E81" s="22">
+        <v>56.064140000000002</v>
+      </c>
+      <c r="F81" s="5">
+        <v>4.3753710000000003</v>
+      </c>
+      <c r="G81" s="24">
+        <v>0.89864100000000002</v>
+      </c>
+      <c r="H81" s="1">
+        <v>22.970182000000001</v>
+      </c>
+      <c r="I81" s="9">
+        <v>496</v>
+      </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="7">
         <v>0.8</v>
       </c>
-      <c r="B82" s="5"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="22"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="24"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="9"/>
+      <c r="B82" s="5">
+        <v>625.241265</v>
+      </c>
+      <c r="C82" s="1">
+        <v>38.092182999999999</v>
+      </c>
+      <c r="D82" s="5">
+        <v>198.742018</v>
+      </c>
+      <c r="E82" s="22">
+        <v>55.875242</v>
+      </c>
+      <c r="F82" s="5">
+        <v>4.3469360000000004</v>
+      </c>
+      <c r="G82" s="24">
+        <v>0.91148399999999996</v>
+      </c>
+      <c r="H82" s="1">
+        <v>23.209274000000001</v>
+      </c>
+      <c r="I82" s="9">
+        <v>487</v>
+      </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="7">
         <v>0.81</v>
       </c>
-      <c r="B83" s="5"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="22"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="24"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="9"/>
+      <c r="B83" s="5">
+        <v>706.45937400000003</v>
+      </c>
+      <c r="C83" s="1">
+        <v>28.34684</v>
+      </c>
+      <c r="D83" s="5">
+        <v>198.787364</v>
+      </c>
+      <c r="E83" s="22">
+        <v>55.681007999999999</v>
+      </c>
+      <c r="F83" s="5">
+        <v>4.3177519999999996</v>
+      </c>
+      <c r="G83" s="24">
+        <v>0.924902</v>
+      </c>
+      <c r="H83" s="1">
+        <v>23.458358</v>
+      </c>
+      <c r="I83" s="9">
+        <v>508</v>
+      </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="7">
         <v>0.82000000000000006</v>
       </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="24"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="9"/>
+      <c r="B84" s="5">
+        <v>952.32548199999997</v>
+      </c>
+      <c r="C84" s="1">
+        <v>34.354761000000003</v>
+      </c>
+      <c r="D84" s="5">
+        <v>198.831298</v>
+      </c>
+      <c r="E84" s="22">
+        <v>55.481124999999999</v>
+      </c>
+      <c r="F84" s="5">
+        <v>4.2877549999999998</v>
+      </c>
+      <c r="G84" s="24">
+        <v>0.93892500000000001</v>
+      </c>
+      <c r="H84" s="1">
+        <v>23.718055</v>
+      </c>
+      <c r="I84" s="9">
+        <v>490</v>
+      </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="7">
         <v>0.83000000000000007</v>
       </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="24"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="9"/>
+      <c r="B85" s="5">
+        <v>667.54977599999995</v>
+      </c>
+      <c r="C85" s="1">
+        <v>20.945136000000002</v>
+      </c>
+      <c r="D85" s="5">
+        <v>198.880258</v>
+      </c>
+      <c r="E85" s="22">
+        <v>55.274959000000003</v>
+      </c>
+      <c r="F85" s="5">
+        <v>4.256996</v>
+      </c>
+      <c r="G85" s="24">
+        <v>0.95371600000000001</v>
+      </c>
+      <c r="H85" s="1">
+        <v>23.990344</v>
+      </c>
+      <c r="I85" s="9">
+        <v>632</v>
+      </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="7">
         <v>0.84</v>
       </c>
-      <c r="B86" s="5"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="22"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="24"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="9"/>
+      <c r="B86" s="5">
+        <v>941.48000300000001</v>
+      </c>
+      <c r="C86" s="1">
+        <v>24.765169</v>
+      </c>
+      <c r="D86" s="5">
+        <v>198.928673</v>
+      </c>
+      <c r="E86" s="22">
+        <v>55.062227</v>
+      </c>
+      <c r="F86" s="5">
+        <v>4.2253210000000001</v>
+      </c>
+      <c r="G86" s="24">
+        <v>0.96924699999999997</v>
+      </c>
+      <c r="H86" s="1">
+        <v>24.275386999999998</v>
+      </c>
+      <c r="I86" s="9">
+        <v>521</v>
+      </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="7">
         <v>0.85</v>
       </c>
-      <c r="B87" s="5"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="5"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="24"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="9"/>
+      <c r="B87" s="5">
+        <v>728.370948</v>
+      </c>
+      <c r="C87" s="1">
+        <v>35.046202000000001</v>
+      </c>
+      <c r="D87" s="5">
+        <v>198.97773000000001</v>
+      </c>
+      <c r="E87" s="22">
+        <v>54.842405999999997</v>
+      </c>
+      <c r="F87" s="5">
+        <v>4.192685</v>
+      </c>
+      <c r="G87" s="24">
+        <v>0.98560999999999999</v>
+      </c>
+      <c r="H87" s="1">
+        <v>24.574521000000001</v>
+      </c>
+      <c r="I87" s="9">
+        <v>478</v>
+      </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="7">
         <v>0.86</v>
       </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="22"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="24"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="9"/>
+      <c r="B88" s="5">
+        <v>394.83374900000001</v>
+      </c>
+      <c r="C88" s="1">
+        <v>13.957420000000001</v>
+      </c>
+      <c r="D88" s="5">
+        <v>199.02983</v>
+      </c>
+      <c r="E88" s="22">
+        <v>54.614851000000002</v>
+      </c>
+      <c r="F88" s="5">
+        <v>4.1590530000000001</v>
+      </c>
+      <c r="G88" s="24">
+        <v>1.002926</v>
+      </c>
+      <c r="H88" s="1">
+        <v>24.889491</v>
+      </c>
+      <c r="I88" s="9">
+        <v>658</v>
+      </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="7">
         <v>0.87</v>
       </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="22"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="24"/>
-      <c r="H89" s="1"/>
-      <c r="I89" s="9"/>
+      <c r="B89" s="5">
+        <v>517.62481500000001</v>
+      </c>
+      <c r="C89" s="1">
+        <v>28.158425999999999</v>
+      </c>
+      <c r="D89" s="5">
+        <v>199.082009</v>
+      </c>
+      <c r="E89" s="22">
+        <v>54.379016999999997</v>
+      </c>
+      <c r="F89" s="5">
+        <v>4.1242919999999996</v>
+      </c>
+      <c r="G89" s="24">
+        <v>1.0212410000000001</v>
+      </c>
+      <c r="H89" s="1">
+        <v>25.221335</v>
+      </c>
+      <c r="I89" s="9">
+        <v>495</v>
+      </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="7">
         <v>0.88</v>
       </c>
-      <c r="B90" s="5"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="22"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="24"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="9"/>
+      <c r="B90" s="5">
+        <v>535.91584799999998</v>
+      </c>
+      <c r="C90" s="1">
+        <v>20.815452000000001</v>
+      </c>
+      <c r="D90" s="5">
+        <v>199.136607</v>
+      </c>
+      <c r="E90" s="22">
+        <v>54.134048</v>
+      </c>
+      <c r="F90" s="5">
+        <v>4.0883390000000004</v>
+      </c>
+      <c r="G90" s="24">
+        <v>1.040708</v>
+      </c>
+      <c r="H90" s="1">
+        <v>25.572293999999999</v>
+      </c>
+      <c r="I90" s="9">
+        <v>650</v>
+      </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="7">
         <v>0.89</v>
       </c>
-      <c r="B91" s="5"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="22"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="24"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="9"/>
+      <c r="B91" s="5">
+        <v>943.33576100000005</v>
+      </c>
+      <c r="C91" s="1">
+        <v>30.292117999999999</v>
+      </c>
+      <c r="D91" s="5">
+        <v>199.19357600000001</v>
+      </c>
+      <c r="E91" s="22">
+        <v>53.879168</v>
+      </c>
+      <c r="F91" s="5">
+        <v>4.0510890000000002</v>
+      </c>
+      <c r="G91" s="24">
+        <v>1.0614509999999999</v>
+      </c>
+      <c r="H91" s="1">
+        <v>25.94435</v>
+      </c>
+      <c r="I91" s="9">
+        <v>493</v>
+      </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="7">
         <v>0.9</v>
       </c>
-      <c r="B92" s="5"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="24"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="9"/>
+      <c r="B92" s="5">
+        <v>412.44972899999999</v>
+      </c>
+      <c r="C92" s="1">
+        <v>47.185645000000001</v>
+      </c>
+      <c r="D92" s="5">
+        <v>199.25020799999999</v>
+      </c>
+      <c r="E92" s="22">
+        <v>53.613464999999998</v>
+      </c>
+      <c r="F92" s="5">
+        <v>4.0123730000000002</v>
+      </c>
+      <c r="G92" s="24">
+        <v>1.083574</v>
+      </c>
+      <c r="H92" s="1">
+        <v>26.339483000000001</v>
+      </c>
+      <c r="I92" s="9">
+        <v>441</v>
+      </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="7">
         <v>0.91</v>
       </c>
-      <c r="B93" s="5"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="22"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="24"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="9"/>
+      <c r="B93" s="5">
+        <v>617.86635000000001</v>
+      </c>
+      <c r="C93" s="1">
+        <v>31.556191999999999</v>
+      </c>
+      <c r="D93" s="5">
+        <v>199.309572</v>
+      </c>
+      <c r="E93" s="22">
+        <v>53.335712000000001</v>
+      </c>
+      <c r="F93" s="5">
+        <v>3.9720900000000001</v>
+      </c>
+      <c r="G93" s="24">
+        <v>1.1073109999999999</v>
+      </c>
+      <c r="H93" s="1">
+        <v>26.761101</v>
+      </c>
+      <c r="I93" s="9">
+        <v>483</v>
+      </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="7">
         <v>0.92</v>
       </c>
-      <c r="B94" s="5"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="24"/>
-      <c r="H94" s="1"/>
-      <c r="I94" s="9"/>
+      <c r="B94" s="5">
+        <v>371.99417999999997</v>
+      </c>
+      <c r="C94" s="1">
+        <v>35.176839000000001</v>
+      </c>
+      <c r="D94" s="5">
+        <v>199.37203099999999</v>
+      </c>
+      <c r="E94" s="22">
+        <v>53.044528999999997</v>
+      </c>
+      <c r="F94" s="5">
+        <v>3.930069</v>
+      </c>
+      <c r="G94" s="24">
+        <v>1.13289</v>
+      </c>
+      <c r="H94" s="1">
+        <v>27.212757</v>
+      </c>
+      <c r="I94" s="9">
+        <v>466</v>
+      </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="7">
         <v>0.93</v>
       </c>
-      <c r="B95" s="5"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="22"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="24"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="9"/>
+      <c r="B95" s="5">
+        <v>601.06899299999998</v>
+      </c>
+      <c r="C95" s="1">
+        <v>29.481888999999999</v>
+      </c>
+      <c r="D95" s="5">
+        <v>199.43623500000001</v>
+      </c>
+      <c r="E95" s="22">
+        <v>52.738425999999997</v>
+      </c>
+      <c r="F95" s="5">
+        <v>3.8860929999999998</v>
+      </c>
+      <c r="G95" s="24">
+        <v>1.1605430000000001</v>
+      </c>
+      <c r="H95" s="1">
+        <v>27.698271999999999</v>
+      </c>
+      <c r="I95" s="9">
+        <v>490</v>
+      </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="7">
         <v>0.94000000000000006</v>
       </c>
-      <c r="B96" s="5"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="22"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="24"/>
-      <c r="H96" s="1"/>
-      <c r="I96" s="9"/>
+      <c r="B96" s="5">
+        <v>874.785482</v>
+      </c>
+      <c r="C96" s="1">
+        <v>26.830487000000002</v>
+      </c>
+      <c r="D96" s="5">
+        <v>199.50298000000001</v>
+      </c>
+      <c r="E96" s="22">
+        <v>52.415422999999997</v>
+      </c>
+      <c r="F96" s="5">
+        <v>3.8399209999999999</v>
+      </c>
+      <c r="G96" s="24">
+        <v>1.1906099999999999</v>
+      </c>
+      <c r="H96" s="1">
+        <v>28.222937000000002</v>
+      </c>
+      <c r="I96" s="9">
+        <v>501</v>
+      </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="7">
         <v>0.95000000000000007</v>
       </c>
-      <c r="B97" s="5"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="22"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="24"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="9"/>
+      <c r="B97" s="5">
+        <v>348.24184300000002</v>
+      </c>
+      <c r="C97" s="1">
+        <v>37.795698999999999</v>
+      </c>
+      <c r="D97" s="5">
+        <v>199.57396600000001</v>
+      </c>
+      <c r="E97" s="22">
+        <v>52.073129999999999</v>
+      </c>
+      <c r="F97" s="5">
+        <v>3.7912810000000001</v>
+      </c>
+      <c r="G97" s="24">
+        <v>1.22353</v>
+      </c>
+      <c r="H97" s="1">
+        <v>28.793399000000001</v>
+      </c>
+      <c r="I97" s="9">
+        <v>444</v>
+      </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="7">
         <v>0.96</v>
       </c>
-      <c r="B98" s="5"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="22"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="24"/>
-      <c r="H98" s="1"/>
-      <c r="I98" s="9"/>
+      <c r="B98" s="5">
+        <v>343.58430800000002</v>
+      </c>
+      <c r="C98" s="1">
+        <v>46.223168000000001</v>
+      </c>
+      <c r="D98" s="5">
+        <v>199.64759000000001</v>
+      </c>
+      <c r="E98" s="22">
+        <v>51.708736000000002</v>
+      </c>
+      <c r="F98" s="5">
+        <v>3.7397849999999999</v>
+      </c>
+      <c r="G98" s="24">
+        <v>1.2597780000000001</v>
+      </c>
+      <c r="H98" s="1">
+        <v>29.417272000000001</v>
+      </c>
+      <c r="I98" s="9">
+        <v>433</v>
+      </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="7">
         <v>0.97</v>
       </c>
-      <c r="B99" s="5"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="22"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="24"/>
-      <c r="H99" s="1"/>
-      <c r="I99" s="9"/>
+      <c r="B99" s="5">
+        <v>206.63069100000001</v>
+      </c>
+      <c r="C99" s="1">
+        <v>35.411918999999997</v>
+      </c>
+      <c r="D99" s="5">
+        <v>199.72557800000001</v>
+      </c>
+      <c r="E99" s="22">
+        <v>51.318489</v>
+      </c>
+      <c r="F99" s="5">
+        <v>3.6849889999999998</v>
+      </c>
+      <c r="G99" s="24">
+        <v>1.3000590000000001</v>
+      </c>
+      <c r="H99" s="1">
+        <v>30.105248</v>
+      </c>
+      <c r="I99" s="9">
+        <v>591</v>
+      </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="7">
         <v>0.98</v>
       </c>
-      <c r="B100" s="5"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="22"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="24"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="9"/>
+      <c r="B100" s="5">
+        <v>793.91892099999995</v>
+      </c>
+      <c r="C100" s="1">
+        <v>15.776319000000001</v>
+      </c>
+      <c r="D100" s="5">
+        <v>199.80882</v>
+      </c>
+      <c r="E100" s="22">
+        <v>50.897646000000002</v>
+      </c>
+      <c r="F100" s="5">
+        <v>3.626309</v>
+      </c>
+      <c r="G100" s="24">
+        <v>1.3452740000000001</v>
+      </c>
+      <c r="H100" s="1">
+        <v>30.87107</v>
+      </c>
+      <c r="I100" s="9">
+        <v>528</v>
+      </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="7">
         <v>0.99</v>
       </c>
-      <c r="B101" s="5"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="22"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="24"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="9"/>
+      <c r="B101" s="5">
+        <v>802.27076399999999</v>
+      </c>
+      <c r="C101" s="1">
+        <v>44.515861999999998</v>
+      </c>
+      <c r="D101" s="5">
+        <v>199.89632399999999</v>
+      </c>
+      <c r="E101" s="22">
+        <v>50.439858000000001</v>
+      </c>
+      <c r="F101" s="5">
+        <v>3.5629300000000002</v>
+      </c>
+      <c r="G101" s="24">
+        <v>1.3966149999999999</v>
+      </c>
+      <c r="H101" s="1">
+        <v>31.733162</v>
+      </c>
+      <c r="I101" s="9">
+        <v>452</v>
+      </c>
     </row>
     <row r="102" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="8">
         <v>1</v>
       </c>
-      <c r="B102" s="6"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="23"/>
-      <c r="F102" s="6"/>
-      <c r="G102" s="25"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="10"/>
+      <c r="B102" s="6">
+        <v>912.52779099999998</v>
+      </c>
+      <c r="C102" s="2">
+        <v>41.681058999999998</v>
+      </c>
+      <c r="D102" s="6">
+        <v>199.98368500000001</v>
+      </c>
+      <c r="E102" s="23">
+        <v>42.733981999999997</v>
+      </c>
+      <c r="F102" s="6">
+        <v>2.5585619999999998</v>
+      </c>
+      <c r="G102" s="25">
+        <v>2.7142369999999998</v>
+      </c>
+      <c r="H102" s="2">
+        <v>52.204096</v>
+      </c>
+      <c r="I102" s="10">
+        <v>435</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>